<commit_message>
2013 download files metadata corrected
</commit_message>
<xml_diff>
--- a/static/download/2013/RP1_APT_ASMA_2013.xlsx
+++ b/static/download/2013/RP1_APT_ASMA_2013.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ASMA_APT" sheetId="1" r:id="rId3"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="177">
   <si>
     <t>Data source</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Meta data</t>
   </si>
   <si>
+    <t>Metadata - Single European Sky Portal</t>
+  </si>
+  <si>
     <t>Release date</t>
   </si>
   <si>
@@ -52,7 +55,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>NSA-PRU-Support@eurocontrol.int</t>
+    <t>pru-support@eurocontrol.int</t>
   </si>
   <si>
     <t>JAN-DEC</t>
@@ -590,8 +593,8 @@
     <font>
       <u/>
       <sz val="9.0"/>
-      <color rgb="FF396EA2"/>
-      <name val="Calibri"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -661,7 +664,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
+    <border/>
     <border>
       <left/>
       <right/>
@@ -796,220 +800,242 @@
   </cellStyleXfs>
   <cellXfs count="79">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="4" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="4" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1018,37 +1044,40 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="19.71"/>
-    <col customWidth="1" min="4" max="4" width="13.86"/>
-    <col customWidth="1" min="5" max="5" width="10.14"/>
-    <col customWidth="1" min="6" max="7" width="11.57"/>
-    <col customWidth="1" min="8" max="8" width="11.0"/>
-    <col customWidth="1" min="9" max="9" width="16.14"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="17.25"/>
+    <col customWidth="1" min="4" max="4" width="12.13"/>
+    <col customWidth="1" min="5" max="5" width="8.88"/>
+    <col customWidth="1" min="6" max="7" width="10.13"/>
+    <col customWidth="1" min="8" max="8" width="9.63"/>
+    <col customWidth="1" min="9" max="9" width="14.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -1067,9 +1096,8 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="str">
-        <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Arrival_sequencing_and_metering_area_(ASMA)_additional_time","ASMA additional time")</f>
-        <v>ASMA additional time</v>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
@@ -1077,22 +1105,22 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="8">
         <v>41758.0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="9">
         <v>41639.0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="12"/>
@@ -1115,60 +1143,60 @@
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="15"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="20">
         <v>101815.0</v>
@@ -1186,16 +1214,16 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="20">
         <v>230263.0</v>
@@ -1213,16 +1241,16 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="20">
         <v>64936.0</v>
@@ -1240,16 +1268,16 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="20">
         <v>54447.0</v>
@@ -1267,16 +1295,16 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="20">
         <v>102238.0</v>
@@ -1294,16 +1322,16 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="20">
         <v>184984.0</v>
@@ -1321,16 +1349,16 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="20">
         <v>50663.0</v>
@@ -1348,16 +1376,16 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="20">
         <v>78354.0</v>
@@ -1375,16 +1403,16 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="20">
         <v>43666.0</v>
@@ -1402,16 +1430,16 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" s="20">
         <v>81757.0</v>
@@ -1429,16 +1457,16 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="20">
         <v>120362.0</v>
@@ -1456,16 +1484,16 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E17" s="20">
         <v>222503.0</v>
@@ -1483,16 +1511,16 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" s="20">
         <v>54003.0</v>
@@ -1510,16 +1538,16 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E19" s="20">
         <v>64194.0</v>
@@ -1537,16 +1565,16 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" s="20">
         <v>212898.0</v>
@@ -1564,16 +1592,16 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E21" s="20">
         <v>82349.0</v>
@@ -1591,16 +1619,16 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" s="20">
         <v>116213.0</v>
@@ -1618,58 +1646,58 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
       <c r="H23" s="25"/>
       <c r="I23" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
       <c r="H24" s="25"/>
       <c r="I24" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" s="20">
         <v>106734.0</v>
@@ -1687,16 +1715,16 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E26" s="20">
         <v>36517.0</v>
@@ -1714,16 +1742,16 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E27" s="20">
         <v>128812.0</v>
@@ -1741,16 +1769,16 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E28" s="20">
         <v>161151.0</v>
@@ -1768,16 +1796,16 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E29" s="20">
         <v>45491.0</v>
@@ -1795,16 +1823,16 @@
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E30" s="20">
         <v>74863.0</v>
@@ -1822,16 +1850,16 @@
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E31" s="20">
         <v>42563.0</v>
@@ -1849,37 +1877,37 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
       <c r="H32" s="25"/>
       <c r="I32" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E33" s="20">
         <v>208548.0</v>
@@ -1897,16 +1925,16 @@
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E34" s="20">
         <v>108761.0</v>
@@ -1924,16 +1952,16 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E35" s="20">
         <v>61541.0</v>
@@ -1951,16 +1979,16 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E36" s="20">
         <v>40598.0</v>
@@ -1978,16 +2006,16 @@
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E37" s="20">
         <v>76513.0</v>
@@ -2005,16 +2033,16 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E38" s="20">
         <v>44794.0</v>
@@ -2032,16 +2060,16 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E39" s="20">
         <v>147166.0</v>
@@ -2059,16 +2087,16 @@
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E40" s="20">
         <v>59732.0</v>
@@ -2086,16 +2114,16 @@
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E41" s="20">
         <v>116024.0</v>
@@ -2113,16 +2141,16 @@
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E42" s="20">
         <v>70125.0</v>
@@ -2140,16 +2168,16 @@
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E43" s="20">
         <v>85009.0</v>
@@ -2167,16 +2195,16 @@
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E44" s="20">
         <v>118293.0</v>
@@ -2224,18 +2252,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="9.0"/>
-    <col customWidth="1" min="6" max="6" width="30.43"/>
+    <col customWidth="1" min="1" max="1" width="12.13"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="9.13"/>
+    <col customWidth="1" min="4" max="4" width="19.13"/>
+    <col customWidth="1" min="5" max="5" width="7.88"/>
+    <col customWidth="1" min="6" max="6" width="26.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2254,29 +2285,28 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="str">
-        <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Arrival_sequencing_and_metering_area_(ASMA)_additional_time","ASMA additional time")</f>
-        <v>ASMA additional time</v>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="8">
         <v>41758.0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="9">
         <v>41639.0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
@@ -2289,29 +2319,29 @@
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="32" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F4" s="34"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="35" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D5" s="36">
         <v>0.0</v>
@@ -2323,13 +2353,13 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D6" s="39">
         <v>2.12515823630473</v>
@@ -2339,13 +2369,13 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D7" s="39">
         <v>2.07060140968231</v>
@@ -2355,11 +2385,11 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="43" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="45"/>
@@ -2470,19 +2500,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
-    <col customWidth="1" min="3" max="3" width="10.43"/>
-    <col customWidth="1" min="4" max="4" width="21.86"/>
-    <col customWidth="1" min="5" max="5" width="12.71"/>
-    <col customWidth="1" min="6" max="6" width="26.0"/>
-    <col customWidth="1" min="7" max="7" width="22.86"/>
+    <col customWidth="1" min="1" max="1" width="11.25"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" min="3" max="3" width="9.13"/>
+    <col customWidth="1" min="4" max="4" width="19.13"/>
+    <col customWidth="1" min="5" max="5" width="11.13"/>
+    <col customWidth="1" min="6" max="6" width="22.75"/>
+    <col customWidth="1" min="7" max="7" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2501,31 +2534,29 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="str">
-        <f>HYPERLINK("http://prudata.webfactional.com/wiki/index.php/Arrival_sequencing_and_metering_area_(ASMA)_additional_time","ASMA additional time")</f>
-        <v>ASMA additional time</v>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G1" s="46"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="8">
         <v>41758.0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="9">
         <v>41639.0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="10" t="str">
-        <f>HYPERLINK("mailto:NSA-PRU-Support@eurocontrol.int","NSA-PRU-Support@eurocontrol.int")</f>
-        <v>NSA-PRU-Support@eurocontrol.int</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="G2" s="47"/>
     </row>
@@ -2549,30 +2580,30 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="51">
@@ -2582,7 +2613,7 @@
         <v>40544.0</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F6" s="36">
         <v>0.0</v>
@@ -2593,7 +2624,7 @@
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="55">
@@ -2603,14 +2634,14 @@
         <v>40575.0</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="59"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="55">
@@ -2620,14 +2651,14 @@
         <v>40603.0</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="59"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="55">
@@ -2637,14 +2668,14 @@
         <v>40634.0</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F9" s="58"/>
       <c r="G9" s="59"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="55">
@@ -2654,14 +2685,14 @@
         <v>40664.0</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F10" s="58"/>
       <c r="G10" s="59"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="55">
@@ -2671,14 +2702,14 @@
         <v>40695.0</v>
       </c>
       <c r="E11" s="57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F11" s="58"/>
       <c r="G11" s="59"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="55">
@@ -2688,14 +2719,14 @@
         <v>40725.0</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F12" s="58"/>
       <c r="G12" s="59"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="55">
@@ -2705,14 +2736,14 @@
         <v>40756.0</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F13" s="58"/>
       <c r="G13" s="59"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="55">
@@ -2722,14 +2753,14 @@
         <v>40787.0</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F14" s="58"/>
       <c r="G14" s="59"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="55">
@@ -2739,14 +2770,14 @@
         <v>40817.0</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F15" s="58"/>
       <c r="G15" s="59"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="55">
@@ -2756,14 +2787,14 @@
         <v>40848.0</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F16" s="58"/>
       <c r="G16" s="59"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="60">
@@ -2773,17 +2804,17 @@
         <v>40878.0</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F17" s="63"/>
       <c r="G17" s="64"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C18" s="51">
         <v>2012.0</v>
@@ -2792,7 +2823,7 @@
         <v>40909.0</v>
       </c>
       <c r="E18" s="53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F18" s="36">
         <v>2.46715442879668</v>
@@ -2801,10 +2832,10 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C19" s="55">
         <v>2012.0</v>
@@ -2813,7 +2844,7 @@
         <v>40940.0</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F19" s="66">
         <v>2.38953363069525</v>
@@ -2822,10 +2853,10 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C20" s="55">
         <v>2012.0</v>
@@ -2834,7 +2865,7 @@
         <v>40969.0</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F20" s="66">
         <v>2.23935112562892</v>
@@ -2843,10 +2874,10 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C21" s="55">
         <v>2012.0</v>
@@ -2855,7 +2886,7 @@
         <v>41000.0</v>
       </c>
       <c r="E21" s="57" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F21" s="66">
         <v>2.19129217001614</v>
@@ -2864,10 +2895,10 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C22" s="55">
         <v>2012.0</v>
@@ -2876,7 +2907,7 @@
         <v>41030.0</v>
       </c>
       <c r="E22" s="57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F22" s="66">
         <v>1.95946265637569</v>
@@ -2885,10 +2916,10 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C23" s="55">
         <v>2012.0</v>
@@ -2897,7 +2928,7 @@
         <v>41061.0</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F23" s="66">
         <v>2.10249593024193</v>
@@ -2906,10 +2937,10 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C24" s="55">
         <v>2012.0</v>
@@ -2918,7 +2949,7 @@
         <v>41091.0</v>
       </c>
       <c r="E24" s="57" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F24" s="66">
         <v>1.82874313458504</v>
@@ -2927,10 +2958,10 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C25" s="55">
         <v>2012.0</v>
@@ -2939,7 +2970,7 @@
         <v>41122.0</v>
       </c>
       <c r="E25" s="57" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F25" s="66">
         <v>1.65224056954627</v>
@@ -2948,10 +2979,10 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C26" s="55">
         <v>2012.0</v>
@@ -2960,7 +2991,7 @@
         <v>41153.0</v>
       </c>
       <c r="E26" s="57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F26" s="66">
         <v>1.99481349870619</v>
@@ -2969,10 +3000,10 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C27" s="55">
         <v>2012.0</v>
@@ -2981,7 +3012,7 @@
         <v>41183.0</v>
       </c>
       <c r="E27" s="57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F27" s="66">
         <v>2.2414690421935</v>
@@ -2990,10 +3021,10 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C28" s="55">
         <v>2012.0</v>
@@ -3002,7 +3033,7 @@
         <v>41214.0</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F28" s="66">
         <v>2.17347849351344</v>
@@ -3011,10 +3042,10 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C29" s="60">
         <v>2012.0</v>
@@ -3023,7 +3054,7 @@
         <v>41244.0</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F29" s="67">
         <v>2.49334109139213</v>
@@ -3032,10 +3063,10 @@
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C30" s="51">
         <v>2013.0</v>
@@ -3044,7 +3075,7 @@
         <v>41275.0</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F30" s="36">
         <v>2.20279591561977</v>
@@ -3053,10 +3084,10 @@
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C31" s="55">
         <v>2013.0</v>
@@ -3065,7 +3096,7 @@
         <v>41306.0</v>
       </c>
       <c r="E31" s="57" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F31" s="66">
         <v>2.24608114571039</v>
@@ -3074,10 +3105,10 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C32" s="55">
         <v>2013.0</v>
@@ -3086,7 +3117,7 @@
         <v>41334.0</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F32" s="66">
         <v>2.30354535517867</v>
@@ -3095,10 +3126,10 @@
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" s="28" t="s">
         <v>166</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>165</v>
       </c>
       <c r="C33" s="55">
         <v>2013.0</v>
@@ -3107,7 +3138,7 @@
         <v>41365.0</v>
       </c>
       <c r="E33" s="57" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F33" s="68">
         <v>2.12333441807296</v>
@@ -3116,10 +3147,10 @@
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="34" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C34" s="55">
         <v>2013.0</v>
@@ -3128,7 +3159,7 @@
         <v>41395.0</v>
       </c>
       <c r="E34" s="57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F34" s="68">
         <v>1.98697273157859</v>
@@ -3137,10 +3168,10 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C35" s="55">
         <v>2013.0</v>
@@ -3149,7 +3180,7 @@
         <v>41426.0</v>
       </c>
       <c r="E35" s="57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F35" s="66">
         <v>2.00001426292883</v>
@@ -3158,10 +3189,10 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C36" s="55">
         <v>2013.0</v>
@@ -3170,7 +3201,7 @@
         <v>41456.0</v>
       </c>
       <c r="E36" s="57" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F36" s="66">
         <v>1.71681998417783</v>
@@ -3179,10 +3210,10 @@
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C37" s="55">
         <v>2013.0</v>
@@ -3191,7 +3222,7 @@
         <v>41487.0</v>
       </c>
       <c r="E37" s="57" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F37" s="66">
         <v>1.64424909789771</v>
@@ -3200,10 +3231,10 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C38" s="55">
         <v>2013.0</v>
@@ -3212,7 +3243,7 @@
         <v>41518.0</v>
       </c>
       <c r="E38" s="57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F38" s="66">
         <v>1.98914998373728</v>
@@ -3221,10 +3252,10 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C39" s="55">
         <v>2013.0</v>
@@ -3233,7 +3264,7 @@
         <v>41548.0</v>
       </c>
       <c r="E39" s="57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F39" s="66">
         <v>2.25445640942794</v>
@@ -3242,10 +3273,10 @@
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C40" s="55">
         <v>2013.0</v>
@@ -3254,7 +3285,7 @@
         <v>41579.0</v>
       </c>
       <c r="E40" s="57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F40" s="66">
         <v>2.13292055629017</v>
@@ -3263,10 +3294,10 @@
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C41" s="60">
         <v>2013.0</v>
@@ -3275,7 +3306,7 @@
         <v>41609.0</v>
       </c>
       <c r="E41" s="62" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F41" s="67">
         <v>2.45585469120083</v>
@@ -3284,7 +3315,7 @@
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B42" s="27"/>
       <c r="C42" s="51">
@@ -3294,14 +3325,14 @@
         <v>41640.0</v>
       </c>
       <c r="E42" s="53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F42" s="69"/>
       <c r="G42" s="65"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B43" s="28"/>
       <c r="C43" s="55">
@@ -3311,14 +3342,14 @@
         <v>41671.0</v>
       </c>
       <c r="E43" s="57" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F43" s="70"/>
       <c r="G43" s="59"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="55">
@@ -3328,14 +3359,14 @@
         <v>41699.0</v>
       </c>
       <c r="E44" s="57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F44" s="70"/>
       <c r="G44" s="59"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B45" s="28"/>
       <c r="C45" s="55">
@@ -3345,14 +3376,14 @@
         <v>41730.0</v>
       </c>
       <c r="E45" s="57" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F45" s="70"/>
       <c r="G45" s="59"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B46" s="28"/>
       <c r="C46" s="55">
@@ -3362,14 +3393,14 @@
         <v>41760.0</v>
       </c>
       <c r="E46" s="57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F46" s="70"/>
       <c r="G46" s="59"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B47" s="28"/>
       <c r="C47" s="55">
@@ -3379,14 +3410,14 @@
         <v>41791.0</v>
       </c>
       <c r="E47" s="57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F47" s="70"/>
       <c r="G47" s="59"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B48" s="28"/>
       <c r="C48" s="55">
@@ -3396,14 +3427,14 @@
         <v>41821.0</v>
       </c>
       <c r="E48" s="57" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F48" s="70"/>
       <c r="G48" s="59"/>
     </row>
     <row r="49" ht="12.0" customHeight="1">
       <c r="A49" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B49" s="28"/>
       <c r="C49" s="55">
@@ -3413,14 +3444,14 @@
         <v>41852.0</v>
       </c>
       <c r="E49" s="57" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F49" s="70"/>
       <c r="G49" s="59"/>
     </row>
     <row r="50" ht="12.0" customHeight="1">
       <c r="A50" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B50" s="28"/>
       <c r="C50" s="55">
@@ -3430,14 +3461,14 @@
         <v>41883.0</v>
       </c>
       <c r="E50" s="57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F50" s="70"/>
       <c r="G50" s="59"/>
     </row>
     <row r="51" ht="12.0" customHeight="1">
       <c r="A51" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="55">
@@ -3447,14 +3478,14 @@
         <v>41913.0</v>
       </c>
       <c r="E51" s="57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F51" s="70"/>
       <c r="G51" s="59"/>
     </row>
     <row r="52" ht="12.0" customHeight="1">
       <c r="A52" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B52" s="28"/>
       <c r="C52" s="55">
@@ -3464,14 +3495,14 @@
         <v>41944.0</v>
       </c>
       <c r="E52" s="57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F52" s="70"/>
       <c r="G52" s="59"/>
     </row>
     <row r="53" ht="12.0" customHeight="1">
       <c r="A53" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="60">
@@ -3481,7 +3512,7 @@
         <v>41974.0</v>
       </c>
       <c r="E53" s="62" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F53" s="71"/>
       <c r="G53" s="64"/>
@@ -3489,38 +3520,40 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F1"/>
-    <hyperlink r:id="rId2" ref="F2"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.57"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="8.0"/>
-    <col customWidth="1" min="4" max="4" width="113.57"/>
-    <col customWidth="1" min="5" max="6" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="9.25"/>
+    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="99.38"/>
+    <col customWidth="1" min="5" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -3528,27 +3561,27 @@
         <v>41320.0</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="76" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="77" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">

</xml_diff>